<commit_message>
test: update test log
</commit_message>
<xml_diff>
--- a/script/测试用例 热.xlsx
+++ b/script/测试用例 热.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21600" windowHeight="10480" activeTab="1"/>
+    <workbookView windowWidth="10800" windowHeight="10480" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="参数配置" sheetId="3" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="127">
   <si>
     <t>模式</t>
   </si>
@@ -357,22 +357,28 @@
     <t>20.33</t>
   </si>
   <si>
+    <t>27，中</t>
+  </si>
+  <si>
     <t>20.5</t>
   </si>
   <si>
-    <t>27，中</t>
-  </si>
-  <si>
     <t>23</t>
   </si>
   <si>
     <t>21.33</t>
   </si>
   <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>0.67</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
     <t>20</t>
-  </si>
-  <si>
-    <t>0.67</t>
   </si>
   <si>
     <t>22.5</t>
@@ -1208,8 +1214,8 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="43" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1252,9 +1258,9 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2474,10 +2480,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AF35"/>
+  <dimension ref="A1:AF37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="T25" sqref="T25"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
@@ -2707,14 +2713,14 @@
       <c r="X4" s="21"/>
       <c r="Y4" s="21"/>
       <c r="Z4" s="21"/>
-      <c r="AA4" s="31"/>
-      <c r="AB4" s="32">
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="31">
         <v>1</v>
       </c>
-      <c r="AC4" s="32"/>
-      <c r="AD4" s="32"/>
-      <c r="AE4" s="33"/>
-      <c r="AF4" s="33"/>
+      <c r="AC4" s="31"/>
+      <c r="AD4" s="31"/>
+      <c r="AE4" s="32"/>
+      <c r="AF4" s="32"/>
     </row>
     <row r="5" s="1" customFormat="1" ht="16.5" spans="1:32">
       <c r="A5" s="8">
@@ -2765,16 +2771,16 @@
       <c r="X5" s="21"/>
       <c r="Y5" s="21"/>
       <c r="Z5" s="21"/>
-      <c r="AA5" s="31"/>
-      <c r="AB5" s="32">
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="31">
         <v>1</v>
       </c>
-      <c r="AC5" s="32">
+      <c r="AC5" s="31">
         <v>2</v>
       </c>
-      <c r="AD5" s="32"/>
-      <c r="AE5" s="33"/>
-      <c r="AF5" s="33"/>
+      <c r="AD5" s="31"/>
+      <c r="AE5" s="32"/>
+      <c r="AF5" s="32"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="16.5" spans="1:32">
       <c r="A6" s="8">
@@ -2831,18 +2837,18 @@
       <c r="X6" s="21"/>
       <c r="Y6" s="21"/>
       <c r="Z6" s="21"/>
-      <c r="AA6" s="31"/>
-      <c r="AB6" s="32">
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="31">
         <v>1</v>
       </c>
-      <c r="AC6" s="32">
+      <c r="AC6" s="31">
         <v>2</v>
       </c>
-      <c r="AD6" s="32">
+      <c r="AD6" s="31">
         <v>3</v>
       </c>
-      <c r="AE6" s="33"/>
-      <c r="AF6" s="33"/>
+      <c r="AE6" s="32"/>
+      <c r="AF6" s="32"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="16.5" spans="1:32">
       <c r="A7" s="8">
@@ -2915,20 +2921,20 @@
       <c r="Z7" s="21">
         <v>0</v>
       </c>
-      <c r="AA7" s="31"/>
-      <c r="AB7" s="32">
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="31">
         <v>1</v>
       </c>
-      <c r="AC7" s="32">
+      <c r="AC7" s="31">
         <v>2</v>
       </c>
-      <c r="AD7" s="32">
+      <c r="AD7" s="31">
         <v>3</v>
       </c>
-      <c r="AE7" s="33">
+      <c r="AE7" s="32">
         <v>4</v>
       </c>
-      <c r="AF7" s="33">
+      <c r="AF7" s="32">
         <v>5</v>
       </c>
     </row>
@@ -3001,20 +3007,20 @@
       <c r="Z8" s="21">
         <v>0</v>
       </c>
-      <c r="AA8" s="31"/>
-      <c r="AB8" s="32">
+      <c r="AA8" s="16"/>
+      <c r="AB8" s="31">
         <v>3</v>
       </c>
-      <c r="AC8" s="32">
+      <c r="AC8" s="31">
         <v>4</v>
       </c>
-      <c r="AD8" s="32">
+      <c r="AD8" s="31">
         <v>5</v>
       </c>
-      <c r="AE8" s="33">
+      <c r="AE8" s="32">
         <v>1</v>
       </c>
-      <c r="AF8" s="33">
+      <c r="AF8" s="32">
         <v>2</v>
       </c>
     </row>
@@ -3085,20 +3091,20 @@
       <c r="Z9" s="21">
         <v>1</v>
       </c>
-      <c r="AA9" s="31"/>
-      <c r="AB9" s="32">
+      <c r="AA9" s="16"/>
+      <c r="AB9" s="31">
         <v>1</v>
       </c>
-      <c r="AC9" s="32">
+      <c r="AC9" s="31">
         <v>4</v>
       </c>
-      <c r="AD9" s="32">
+      <c r="AD9" s="31">
         <v>5</v>
       </c>
-      <c r="AE9" s="33">
+      <c r="AE9" s="32">
         <v>2</v>
       </c>
-      <c r="AF9" s="33">
+      <c r="AF9" s="32">
         <v>3</v>
       </c>
     </row>
@@ -3167,20 +3173,20 @@
       <c r="Z10" s="21">
         <v>1</v>
       </c>
-      <c r="AA10" s="31"/>
-      <c r="AB10" s="32">
+      <c r="AA10" s="16"/>
+      <c r="AB10" s="31">
         <v>1</v>
       </c>
-      <c r="AC10" s="32">
+      <c r="AC10" s="31">
         <v>5</v>
       </c>
-      <c r="AD10" s="32">
+      <c r="AD10" s="31">
         <v>2</v>
       </c>
-      <c r="AE10" s="33">
+      <c r="AE10" s="32">
         <v>3</v>
       </c>
-      <c r="AF10" s="33">
+      <c r="AF10" s="32">
         <v>4</v>
       </c>
     </row>
@@ -3251,20 +3257,20 @@
       <c r="Z11" s="21">
         <v>1</v>
       </c>
-      <c r="AA11" s="31"/>
-      <c r="AB11" s="32">
+      <c r="AA11" s="16"/>
+      <c r="AB11" s="31">
         <v>1</v>
       </c>
-      <c r="AC11" s="32">
+      <c r="AC11" s="31">
         <v>5</v>
       </c>
-      <c r="AD11" s="32">
+      <c r="AD11" s="31">
         <v>2</v>
       </c>
-      <c r="AE11" s="33">
+      <c r="AE11" s="32">
         <v>3</v>
       </c>
-      <c r="AF11" s="33">
+      <c r="AF11" s="32">
         <v>4</v>
       </c>
     </row>
@@ -3333,20 +3339,20 @@
       <c r="Z12" s="21">
         <v>1</v>
       </c>
-      <c r="AA12" s="31"/>
-      <c r="AB12" s="32">
+      <c r="AA12" s="16"/>
+      <c r="AB12" s="31">
         <v>1</v>
       </c>
-      <c r="AC12" s="32">
+      <c r="AC12" s="31">
         <v>5</v>
       </c>
-      <c r="AD12" s="32">
+      <c r="AD12" s="31">
         <v>3</v>
       </c>
-      <c r="AE12" s="33">
+      <c r="AE12" s="32">
         <v>2</v>
       </c>
-      <c r="AF12" s="33">
+      <c r="AF12" s="32">
         <v>4</v>
       </c>
     </row>
@@ -3419,20 +3425,20 @@
       <c r="Z13" s="21">
         <v>1</v>
       </c>
-      <c r="AA13" s="31"/>
-      <c r="AB13" s="32">
+      <c r="AA13" s="16"/>
+      <c r="AB13" s="31">
         <v>1</v>
       </c>
-      <c r="AC13" s="32">
+      <c r="AC13" s="31">
         <v>5</v>
       </c>
-      <c r="AD13" s="32">
+      <c r="AD13" s="31">
         <v>3</v>
       </c>
-      <c r="AE13" s="33">
+      <c r="AE13" s="32">
         <v>2</v>
       </c>
-      <c r="AF13" s="33">
+      <c r="AF13" s="32">
         <v>4</v>
       </c>
     </row>
@@ -3501,20 +3507,20 @@
       <c r="Z14" s="21">
         <v>1</v>
       </c>
-      <c r="AA14" s="31"/>
-      <c r="AB14" s="32">
+      <c r="AA14" s="16"/>
+      <c r="AB14" s="31">
         <v>1</v>
       </c>
-      <c r="AC14" s="32">
+      <c r="AC14" s="31">
         <v>5</v>
       </c>
-      <c r="AD14" s="32">
+      <c r="AD14" s="31">
         <v>4</v>
       </c>
-      <c r="AE14" s="33">
+      <c r="AE14" s="32">
         <v>2</v>
       </c>
-      <c r="AF14" s="33">
+      <c r="AF14" s="32">
         <v>3</v>
       </c>
     </row>
@@ -3585,20 +3591,20 @@
       <c r="Z15" s="21">
         <v>1</v>
       </c>
-      <c r="AA15" s="31"/>
-      <c r="AB15" s="32">
+      <c r="AA15" s="16"/>
+      <c r="AB15" s="31">
         <v>1</v>
       </c>
-      <c r="AC15" s="32">
+      <c r="AC15" s="31">
         <v>5</v>
       </c>
-      <c r="AD15" s="32">
+      <c r="AD15" s="31">
         <v>4</v>
       </c>
-      <c r="AE15" s="33">
+      <c r="AE15" s="32">
         <v>2</v>
       </c>
-      <c r="AF15" s="33">
+      <c r="AF15" s="32">
         <v>3</v>
       </c>
     </row>
@@ -3669,20 +3675,20 @@
       <c r="Z16" s="21">
         <v>0.5</v>
       </c>
-      <c r="AA16" s="31"/>
-      <c r="AB16" s="32">
+      <c r="AA16" s="16"/>
+      <c r="AB16" s="31">
         <v>1</v>
       </c>
-      <c r="AC16" s="32">
+      <c r="AC16" s="31">
         <v>2</v>
       </c>
-      <c r="AD16" s="32">
+      <c r="AD16" s="31">
         <v>2</v>
       </c>
-      <c r="AE16" s="33">
+      <c r="AE16" s="32">
         <v>3</v>
       </c>
-      <c r="AF16" s="33">
+      <c r="AF16" s="32">
         <v>4</v>
       </c>
     </row>
@@ -3751,20 +3757,20 @@
       <c r="Z17" s="21">
         <v>0.5</v>
       </c>
-      <c r="AA17" s="31"/>
-      <c r="AB17" s="32">
+      <c r="AA17" s="16"/>
+      <c r="AB17" s="31">
         <v>1</v>
       </c>
-      <c r="AC17" s="32">
+      <c r="AC17" s="31">
         <v>2</v>
       </c>
-      <c r="AD17" s="32">
+      <c r="AD17" s="31">
         <v>3</v>
       </c>
-      <c r="AE17" s="33">
+      <c r="AE17" s="32">
         <v>4</v>
       </c>
-      <c r="AF17" s="33">
+      <c r="AF17" s="32">
         <v>5</v>
       </c>
     </row>
@@ -3837,20 +3843,20 @@
       <c r="Z18" s="21">
         <v>0</v>
       </c>
-      <c r="AA18" s="31"/>
-      <c r="AB18" s="32">
+      <c r="AA18" s="16"/>
+      <c r="AB18" s="31">
         <v>2</v>
       </c>
-      <c r="AC18" s="32">
+      <c r="AC18" s="31">
         <v>4</v>
       </c>
-      <c r="AD18" s="32">
+      <c r="AD18" s="31">
         <v>5</v>
       </c>
-      <c r="AE18" s="33">
+      <c r="AE18" s="32">
         <v>3</v>
       </c>
-      <c r="AF18" s="33"/>
+      <c r="AF18" s="32"/>
     </row>
     <row r="19" s="1" customFormat="1" ht="16.5" spans="1:32">
       <c r="A19" s="8">
@@ -3913,20 +3919,20 @@
       <c r="Z19" s="21">
         <v>0.5</v>
       </c>
-      <c r="AA19" s="31"/>
-      <c r="AB19" s="32">
+      <c r="AA19" s="16"/>
+      <c r="AB19" s="31">
         <v>2</v>
       </c>
-      <c r="AC19" s="32">
+      <c r="AC19" s="31">
         <v>4</v>
       </c>
-      <c r="AD19" s="32">
+      <c r="AD19" s="31">
         <v>5</v>
       </c>
-      <c r="AE19" s="33">
+      <c r="AE19" s="32">
         <v>3</v>
       </c>
-      <c r="AF19" s="33"/>
+      <c r="AF19" s="32"/>
     </row>
     <row r="20" s="1" customFormat="1" ht="16.5" spans="1:32">
       <c r="A20" s="8">
@@ -3991,18 +3997,18 @@
       <c r="Z20" s="21">
         <v>0.5</v>
       </c>
-      <c r="AA20" s="31"/>
-      <c r="AB20" s="32">
+      <c r="AA20" s="16"/>
+      <c r="AB20" s="31">
         <v>2</v>
       </c>
-      <c r="AC20" s="32">
+      <c r="AC20" s="31">
         <v>3</v>
       </c>
-      <c r="AD20" s="32">
+      <c r="AD20" s="31">
         <v>4</v>
       </c>
-      <c r="AE20" s="33"/>
-      <c r="AF20" s="33"/>
+      <c r="AE20" s="32"/>
+      <c r="AF20" s="32"/>
     </row>
     <row r="21" s="1" customFormat="1" ht="16.5" spans="1:32">
       <c r="A21" s="8">
@@ -4063,18 +4069,18 @@
       <c r="X21" s="23"/>
       <c r="Y21" s="23"/>
       <c r="Z21" s="23"/>
-      <c r="AA21" s="31"/>
-      <c r="AB21" s="32">
+      <c r="AA21" s="16"/>
+      <c r="AB21" s="31">
         <v>2</v>
       </c>
-      <c r="AC21" s="32">
+      <c r="AC21" s="31">
         <v>3</v>
       </c>
-      <c r="AD21" s="32">
+      <c r="AD21" s="31">
         <v>4</v>
       </c>
-      <c r="AE21" s="33"/>
-      <c r="AF21" s="33"/>
+      <c r="AE21" s="32"/>
+      <c r="AF21" s="32"/>
     </row>
     <row r="22" s="1" customFormat="1" ht="16.5" spans="1:32">
       <c r="A22" s="8">
@@ -4140,20 +4146,20 @@
       <c r="X22" s="23"/>
       <c r="Y22" s="23"/>
       <c r="Z22" s="23"/>
-      <c r="AA22" s="31"/>
-      <c r="AB22" s="32">
+      <c r="AA22" s="16"/>
+      <c r="AB22" s="31">
         <v>1</v>
       </c>
-      <c r="AC22" s="32">
+      <c r="AC22" s="31">
         <v>2</v>
       </c>
-      <c r="AD22" s="32">
+      <c r="AD22" s="31">
         <v>3</v>
       </c>
-      <c r="AE22" s="33">
+      <c r="AE22" s="32">
         <v>4</v>
       </c>
-      <c r="AF22" s="33"/>
+      <c r="AF22" s="32"/>
     </row>
     <row r="23" s="1" customFormat="1" ht="16.5" spans="1:32">
       <c r="A23" s="8">
@@ -4200,10 +4206,10 @@
         <v>59</v>
       </c>
       <c r="S23" s="28" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="T23" s="28" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="U23" s="28"/>
       <c r="V23" s="28" t="s">
@@ -4215,20 +4221,20 @@
       <c r="X23" s="23"/>
       <c r="Y23" s="23"/>
       <c r="Z23" s="23"/>
-      <c r="AA23" s="31"/>
-      <c r="AB23" s="32">
+      <c r="AA23" s="16"/>
+      <c r="AB23" s="31">
         <v>1</v>
       </c>
-      <c r="AC23" s="32">
+      <c r="AC23" s="31">
         <v>2</v>
       </c>
-      <c r="AD23" s="32">
+      <c r="AD23" s="31">
         <v>3</v>
       </c>
-      <c r="AE23" s="33">
+      <c r="AE23" s="32">
         <v>4</v>
       </c>
-      <c r="AF23" s="33"/>
+      <c r="AF23" s="32"/>
     </row>
     <row r="24" s="1" customFormat="1" ht="16.5" spans="1:32">
       <c r="A24" s="8">
@@ -4236,7 +4242,7 @@
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
@@ -4244,7 +4250,7 @@
         <v>93</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H24" s="14" t="s">
         <v>100</v>
@@ -4283,14 +4289,14 @@
         <v>113</v>
       </c>
       <c r="T24" s="28" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="U24" s="28"/>
       <c r="V24" s="28" t="s">
         <v>105</v>
       </c>
       <c r="W24" s="23" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="X24" s="23" t="s">
         <v>100</v>
@@ -4299,20 +4305,20 @@
       <c r="Z24" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="AA24" s="31"/>
-      <c r="AB24" s="32">
+      <c r="AA24" s="16"/>
+      <c r="AB24" s="31">
         <v>1</v>
       </c>
-      <c r="AC24" s="32">
+      <c r="AC24" s="31">
         <v>2</v>
       </c>
-      <c r="AD24" s="32">
+      <c r="AD24" s="31">
         <v>3</v>
       </c>
-      <c r="AE24" s="33">
+      <c r="AE24" s="32">
         <v>4</v>
       </c>
-      <c r="AF24" s="33">
+      <c r="AF24" s="32">
         <v>5</v>
       </c>
     </row>
@@ -4360,10 +4366,10 @@
         <v>114</v>
       </c>
       <c r="S25" s="28" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="T25" s="28" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="U25" s="28" t="s">
         <v>10</v>
@@ -4372,7 +4378,7 @@
         <v>105</v>
       </c>
       <c r="W25" s="23" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="X25" s="23" t="s">
         <v>100</v>
@@ -4381,20 +4387,20 @@
       <c r="Z25" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="AA25" s="31"/>
-      <c r="AB25" s="32">
+      <c r="AA25" s="16"/>
+      <c r="AB25" s="31">
         <v>1</v>
       </c>
-      <c r="AC25" s="32">
+      <c r="AC25" s="31">
         <v>2</v>
       </c>
-      <c r="AD25" s="32">
+      <c r="AD25" s="31">
         <v>4</v>
       </c>
-      <c r="AE25" s="33">
+      <c r="AE25" s="32">
         <v>5</v>
       </c>
-      <c r="AF25" s="33"/>
+      <c r="AF25" s="32"/>
     </row>
     <row r="26" ht="16.5" spans="1:32">
       <c r="A26" s="8">
@@ -4406,7 +4412,7 @@
       <c r="E26" s="12"/>
       <c r="F26" s="12"/>
       <c r="G26" s="14" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H26" s="14" t="s">
         <v>100</v>
@@ -4441,7 +4447,7 @@
         <v>113</v>
       </c>
       <c r="T26" s="28" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="U26" s="28" t="s">
         <v>10</v>
@@ -4461,18 +4467,18 @@
       <c r="Z26" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="AA26" s="16"/>
-      <c r="AB26" s="32">
+      <c r="AA26" s="33"/>
+      <c r="AB26" s="31">
         <v>1</v>
       </c>
-      <c r="AC26" s="32">
+      <c r="AC26" s="31">
         <v>4</v>
       </c>
-      <c r="AD26" s="32">
+      <c r="AD26" s="31">
         <v>5</v>
       </c>
-      <c r="AE26" s="33"/>
-      <c r="AF26" s="33"/>
+      <c r="AE26" s="32"/>
+      <c r="AF26" s="32"/>
     </row>
     <row r="27" ht="16.5" spans="1:32">
       <c r="A27" s="8">
@@ -4484,7 +4490,7 @@
       <c r="E27" s="12"/>
       <c r="F27" s="12"/>
       <c r="G27" s="14" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H27" s="14" t="s">
         <v>100</v>
@@ -4496,7 +4502,7 @@
         <v>59</v>
       </c>
       <c r="K27" s="23" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="L27" s="23" t="s">
         <v>102</v>
@@ -4518,17 +4524,17 @@
         <v>105</v>
       </c>
       <c r="S27" s="28" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="T27" s="28" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="U27" s="28"/>
       <c r="V27" s="28" t="s">
         <v>98</v>
       </c>
       <c r="W27" s="23" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="X27" s="23" t="s">
         <v>100</v>
@@ -4539,20 +4545,20 @@
       <c r="Z27" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="AA27" s="16"/>
-      <c r="AB27" s="32">
+      <c r="AA27" s="33"/>
+      <c r="AB27" s="31">
         <v>1</v>
       </c>
-      <c r="AC27" s="32">
+      <c r="AC27" s="31">
         <v>3</v>
       </c>
-      <c r="AD27" s="32">
+      <c r="AD27" s="31">
         <v>5</v>
       </c>
-      <c r="AE27" s="33">
+      <c r="AE27" s="32">
         <v>4</v>
       </c>
-      <c r="AF27" s="33"/>
+      <c r="AF27" s="32"/>
     </row>
     <row r="28" ht="16.5" spans="1:32">
       <c r="A28" s="8">
@@ -4605,7 +4611,7 @@
         <v>113</v>
       </c>
       <c r="T28" s="28" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="U28" s="28" t="s">
         <v>10</v>
@@ -4614,7 +4620,7 @@
         <v>105</v>
       </c>
       <c r="W28" s="23" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="X28" s="23" t="s">
         <v>100</v>
@@ -4623,16 +4629,16 @@
       <c r="Z28" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="AA28" s="16"/>
-      <c r="AB28" s="32">
+      <c r="AA28" s="33"/>
+      <c r="AB28" s="31">
         <v>2</v>
       </c>
-      <c r="AC28" s="32">
+      <c r="AC28" s="31">
         <v>4</v>
       </c>
-      <c r="AD28" s="32"/>
-      <c r="AE28" s="33"/>
-      <c r="AF28" s="33"/>
+      <c r="AD28" s="31"/>
+      <c r="AE28" s="32"/>
+      <c r="AF28" s="32"/>
     </row>
     <row r="29" ht="16.5" spans="1:32">
       <c r="A29" s="8">
@@ -4666,10 +4672,10 @@
       <c r="Q29" s="24"/>
       <c r="R29" s="24"/>
       <c r="S29" s="28" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="T29" s="28" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="U29" s="28" t="s">
         <v>10</v>
@@ -4681,16 +4687,16 @@
       <c r="X29" s="23"/>
       <c r="Y29" s="23"/>
       <c r="Z29" s="23"/>
-      <c r="AA29" s="16"/>
-      <c r="AB29" s="32"/>
-      <c r="AC29" s="32"/>
-      <c r="AD29" s="32"/>
-      <c r="AE29" s="33"/>
-      <c r="AF29" s="33"/>
+      <c r="AA29" s="33"/>
+      <c r="AB29" s="31"/>
+      <c r="AC29" s="31"/>
+      <c r="AD29" s="31"/>
+      <c r="AE29" s="32"/>
+      <c r="AF29" s="32"/>
     </row>
     <row r="30" ht="16.5" spans="1:32">
       <c r="A30" s="8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -4701,7 +4707,7 @@
       <c r="H30" s="14"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="K30" s="23"/>
       <c r="L30" s="23"/>
@@ -4713,28 +4719,34 @@
       <c r="P30" s="24"/>
       <c r="Q30" s="24"/>
       <c r="R30" s="24" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="S30" s="28"/>
       <c r="T30" s="28"/>
       <c r="U30" s="28"/>
       <c r="V30" s="28" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="W30" s="23"/>
       <c r="X30" s="23"/>
       <c r="Y30" s="23"/>
       <c r="Z30" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="AA30" s="16"/>
-      <c r="AB30" s="32"/>
-      <c r="AC30" s="32"/>
-      <c r="AD30" s="32"/>
-      <c r="AE30" s="33"/>
-      <c r="AF30" s="33"/>
-    </row>
-    <row r="31" spans="7:32">
+        <v>124</v>
+      </c>
+      <c r="AA30" s="33"/>
+      <c r="AB30" s="31"/>
+      <c r="AC30" s="31"/>
+      <c r="AD30" s="31"/>
+      <c r="AE30" s="32"/>
+      <c r="AF30" s="32"/>
+    </row>
+    <row r="31" ht="16.5" spans="1:32">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
       <c r="G31" s="15"/>
       <c r="H31" s="15"/>
       <c r="I31" s="15"/>
@@ -4759,13 +4771,18 @@
       <c r="AB31" s="16"/>
       <c r="AC31" s="16"/>
       <c r="AD31" s="16"/>
-      <c r="AE31" s="16"/>
-      <c r="AF31" s="16"/>
-    </row>
-    <row r="32" spans="1:32">
-      <c r="A32" s="2" t="s">
-        <v>123</v>
-      </c>
+      <c r="AE31" s="33"/>
+      <c r="AF31" s="33"/>
+    </row>
+    <row r="32" ht="16.5" spans="1:32">
+      <c r="A32" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
       <c r="G32" s="15"/>
       <c r="H32" s="15"/>
       <c r="I32" s="15"/>
@@ -4790,13 +4807,18 @@
       <c r="AB32" s="16"/>
       <c r="AC32" s="16"/>
       <c r="AD32" s="16"/>
-      <c r="AE32" s="16"/>
-      <c r="AF32" s="16"/>
-    </row>
-    <row r="33" spans="1:32">
-      <c r="A33" s="2" t="s">
-        <v>124</v>
-      </c>
+      <c r="AE32" s="33"/>
+      <c r="AF32" s="33"/>
+    </row>
+    <row r="33" ht="16.5" spans="1:32">
+      <c r="A33" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
       <c r="G33" s="15"/>
       <c r="H33" s="15"/>
       <c r="I33" s="15"/>
@@ -4821,10 +4843,16 @@
       <c r="AB33" s="16"/>
       <c r="AC33" s="16"/>
       <c r="AD33" s="16"/>
-      <c r="AE33" s="16"/>
-      <c r="AF33" s="16"/>
-    </row>
-    <row r="34" spans="7:32">
+      <c r="AE33" s="33"/>
+      <c r="AF33" s="33"/>
+    </row>
+    <row r="34" ht="16.5" spans="1:32">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
       <c r="G34" s="15"/>
       <c r="H34" s="15"/>
       <c r="I34" s="15"/>
@@ -4849,10 +4877,16 @@
       <c r="AB34" s="16"/>
       <c r="AC34" s="16"/>
       <c r="AD34" s="16"/>
-      <c r="AE34" s="16"/>
-      <c r="AF34" s="16"/>
-    </row>
-    <row r="35" spans="7:32">
+      <c r="AE34" s="33"/>
+      <c r="AF34" s="33"/>
+    </row>
+    <row r="35" ht="16.5" spans="1:32">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
       <c r="G35" s="16"/>
       <c r="H35" s="16"/>
       <c r="I35" s="16"/>
@@ -4877,8 +4911,72 @@
       <c r="AB35" s="16"/>
       <c r="AC35" s="16"/>
       <c r="AD35" s="16"/>
-      <c r="AE35" s="16"/>
-      <c r="AF35" s="16"/>
+      <c r="AE35" s="33"/>
+      <c r="AF35" s="33"/>
+    </row>
+    <row r="36" ht="16.5" spans="1:30">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
+      <c r="AA36" s="1"/>
+      <c r="AB36" s="1"/>
+      <c r="AC36" s="1"/>
+      <c r="AD36" s="1"/>
+    </row>
+    <row r="37" ht="16.5" spans="1:30">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+      <c r="Z37" s="1"/>
+      <c r="AA37" s="1"/>
+      <c r="AB37" s="1"/>
+      <c r="AC37" s="1"/>
+      <c r="AD37" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>